<commit_message>
membuat fitur alokasi mitra
</commit_message>
<xml_diff>
--- a/public/template_excel/template mitra.xlsx
+++ b/public/template_excel/template mitra.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\KULIAH\Magang\SIAP_project\SIAP_bps\public\template_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5651FAF-C583-44AA-8AB3-CDD3EFEAAC84}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3591507-0BA0-4B27-B8F6-9377B011C2F4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4461D531-C442-4DF0-AFD6-87698AEF49A2}"/>
   </bookViews>
@@ -32,9 +32,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>idsobat</t>
-  </si>
-  <si>
     <t>nik</t>
   </si>
   <si>
@@ -48,6 +45,9 @@
   </si>
   <si>
     <t>jenis_kelamin</t>
+  </si>
+  <si>
+    <t>sobat_id</t>
   </si>
 </sst>
 </file>
@@ -402,7 +402,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -412,22 +412,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>